<commit_message>
Starting to converge to my solution
</commit_message>
<xml_diff>
--- a/Excel-BI-Excel-Challenge-412.xlsx
+++ b/Excel-BI-Excel-Challenge-412.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5A5FBC3-8C1E-423E-BFB4-21DC761B91DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{F5A5FBC3-8C1E-423E-BFB4-21DC761B91DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EE7860A-ECA7-491A-91FD-3AABE20DF8D6}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="11" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>FROM:</t>
   </si>
@@ -169,6 +171,12 @@
   </si>
   <si>
     <t>His solution</t>
+  </si>
+  <si>
+    <t>My Solution</t>
+  </si>
+  <si>
+    <t>Checks out</t>
   </si>
 </sst>
 </file>
@@ -295,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +380,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -420,7 +434,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -434,7 +448,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -442,6 +455,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -1120,7 +1135,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1412,10 +1427,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1462,22 +1477,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="str" cm="1">
+      <c r="F9" s="13" t="str" cm="1">
         <f t="array" ref="F9:G18">_xlfn.REDUCE(B9:C9,A10:A18,_xlfn.LAMBDA(_xlpm.c,_xlpm.v,_xlfn.VSTACK(_xlpm.c,_xlfn.REDUCE(_xlpm.v,_xlfn.SEQUENCE(20),_xlfn.LAMBDA(_xlpm.a,_xlpm.n,_xlfn.LET(_xlpm.b,SUM(MID(_xlpm.a,_xlfn.SEQUENCE(LEN(_xlpm.a)),1)^2),IF((_xlpm.b&lt;10)*_xlpm.n,_xlfn.HSTACK(_xlpm.b,_xlpm.n),IF(COUNT(_xlpm.a)&gt;1,_xlpm.a,_xlpm.b))))))))</f>
         <v>Final Digit</v>
       </c>
@@ -1653,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>999999</v>
       </c>
@@ -1676,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3078682</v>
       </c>
@@ -1697,6 +1712,329 @@
       </c>
       <c r="J18" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22:F30">_xlfn.MAP(A10:A18,_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>36</v>
+      </c>
+      <c r="G22" cm="1">
+        <f t="array" ref="G22:G30">_xlfn.MAP(_xlfn.ANCHORARRAY(F22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>45</v>
+      </c>
+      <c r="H22" cm="1">
+        <f t="array" ref="H22:H30">_xlfn.MAP(_xlfn.ANCHORARRAY(G22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>41</v>
+      </c>
+      <c r="I22" cm="1">
+        <f t="array" ref="I22:I30">_xlfn.MAP(_xlfn.ANCHORARRAY(H22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>17</v>
+      </c>
+      <c r="J22" cm="1">
+        <f t="array" ref="J22:J30">_xlfn.MAP(_xlfn.ANCHORARRAY(I22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>50</v>
+      </c>
+      <c r="K22" cm="1">
+        <f t="array" ref="K22:K30">_xlfn.MAP(_xlfn.ANCHORARRAY(J22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>25</v>
+      </c>
+      <c r="L22" cm="1">
+        <f t="array" ref="L22:L30">_xlfn.MAP(_xlfn.ANCHORARRAY(K22),_xlfn.LAMBDA(_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.x,_xlfn.SEQUENCE(LEN(_xlpm.x)),1))^2)))</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <v>85</v>
+      </c>
+      <c r="J23">
+        <v>89</v>
+      </c>
+      <c r="K23">
+        <v>145</v>
+      </c>
+      <c r="L23">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="18">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>25</v>
+      </c>
+      <c r="H24">
+        <v>29</v>
+      </c>
+      <c r="I24">
+        <v>85</v>
+      </c>
+      <c r="J24">
+        <v>89</v>
+      </c>
+      <c r="K24">
+        <v>145</v>
+      </c>
+      <c r="L24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>29</v>
+      </c>
+      <c r="G25">
+        <v>85</v>
+      </c>
+      <c r="H25">
+        <v>89</v>
+      </c>
+      <c r="I25">
+        <v>145</v>
+      </c>
+      <c r="J25">
+        <v>42</v>
+      </c>
+      <c r="K25">
+        <v>20</v>
+      </c>
+      <c r="L25" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>151</v>
+      </c>
+      <c r="G26">
+        <v>27</v>
+      </c>
+      <c r="H26">
+        <v>53</v>
+      </c>
+      <c r="I26">
+        <v>34</v>
+      </c>
+      <c r="J26">
+        <v>25</v>
+      </c>
+      <c r="K26">
+        <v>29</v>
+      </c>
+      <c r="L26">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>128</v>
+      </c>
+      <c r="G27">
+        <v>69</v>
+      </c>
+      <c r="H27">
+        <v>117</v>
+      </c>
+      <c r="I27">
+        <v>51</v>
+      </c>
+      <c r="J27">
+        <v>26</v>
+      </c>
+      <c r="K27">
+        <v>40</v>
+      </c>
+      <c r="L27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>197</v>
+      </c>
+      <c r="G28">
+        <v>131</v>
+      </c>
+      <c r="H28">
+        <v>11</v>
+      </c>
+      <c r="I28" s="18">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>16</v>
+      </c>
+      <c r="L28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>486</v>
+      </c>
+      <c r="G29">
+        <v>116</v>
+      </c>
+      <c r="H29">
+        <v>38</v>
+      </c>
+      <c r="I29">
+        <v>73</v>
+      </c>
+      <c r="J29">
+        <v>58</v>
+      </c>
+      <c r="K29">
+        <v>89</v>
+      </c>
+      <c r="L29">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>226</v>
+      </c>
+      <c r="G30">
+        <v>44</v>
+      </c>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>13</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30" s="18">
+        <v>1</v>
+      </c>
+      <c r="L30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" cm="1">
+        <f t="array" ref="F33:F52">_xlfn.SCAN(A10,_xlfn.SEQUENCE(20),_xlfn.LAMBDA(_xlpm.a,_xlpm.x,SUM(TRANSPOSE(MID(_xlpm.a,_xlfn.SEQUENCE(LEN(_xlpm.a)),1))^2)))</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1889,19 +2227,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="13">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1909,11 +2243,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1921,19 +2254,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1941,11 +2270,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1953,19 +2281,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1973,11 +2297,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1985,13 +2308,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>